<commit_message>
Adds a boolean lever to use a non BAU ZEV qualifying vehicle data file and converts qualifying vehicles to a time-series variable instead of a constant.
</commit_message>
<xml_diff>
--- a/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
+++ b/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\VTQaZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\VTQaZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D282A55-84E0-4AAE-A63D-CAEA0DE00BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DC1478-33EC-495A-BDBA-446C75BCAD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12105" yWindow="2595" windowWidth="29940" windowHeight="20805" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
+    <workbookView xWindow="14505" yWindow="6405" windowWidth="28800" windowHeight="15600" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>VTQaZ Vehicle Technologies Qualifying as ZEVs</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>none needed</t>
-  </si>
-  <si>
-    <t>Does this vehicle technology qualify as a ZEV?</t>
   </si>
   <si>
     <t>hydrogen vehicle</t>
@@ -472,76 +469,798 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>2020</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2022</v>
+      </c>
+      <c r="E1">
+        <v>2023</v>
+      </c>
+      <c r="F1">
+        <v>2024</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2026</v>
+      </c>
+      <c r="I1">
+        <v>2027</v>
+      </c>
+      <c r="J1">
+        <v>2028</v>
+      </c>
+      <c r="K1">
+        <v>2029</v>
+      </c>
+      <c r="L1">
+        <v>2030</v>
+      </c>
+      <c r="M1">
+        <v>2031</v>
+      </c>
+      <c r="N1">
+        <v>2032</v>
+      </c>
+      <c r="O1">
+        <v>2033</v>
+      </c>
+      <c r="P1">
+        <v>2034</v>
+      </c>
+      <c r="Q1">
+        <v>2035</v>
+      </c>
+      <c r="R1">
+        <v>2036</v>
+      </c>
+      <c r="S1">
+        <v>2037</v>
+      </c>
+      <c r="T1">
+        <v>2038</v>
+      </c>
+      <c r="U1">
+        <v>2039</v>
+      </c>
+      <c r="V1">
+        <v>2040</v>
+      </c>
+      <c r="W1">
+        <v>2041</v>
+      </c>
+      <c r="X1">
+        <v>2042</v>
+      </c>
+      <c r="Y1">
+        <v>2043</v>
+      </c>
+      <c r="Z1">
+        <v>2044</v>
+      </c>
+      <c r="AA1">
+        <v>2045</v>
+      </c>
+      <c r="AB1">
+        <v>2046</v>
+      </c>
+      <c r="AC1">
+        <v>2047</v>
+      </c>
+      <c r="AD1">
+        <v>2048</v>
+      </c>
+      <c r="AE1">
+        <v>2049</v>
+      </c>
+      <c r="AF1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
       <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to NDC scenario to use non BAU ZEV schedule and updates to policy schedules to disallow PHEV starting in 2034 in the Non BAU file.
</commit_message>
<xml_diff>
--- a/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
+++ b/InputData/trans/VTQaZ/Veh Techs Qualifying as ZEVs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\VTQaZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DC1478-33EC-495A-BDBA-446C75BCAD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2410B116-F72B-481A-8955-3426D2F171F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="6405" windowWidth="28800" windowHeight="15600" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{7166B4F5-29DF-47A7-8501-7E54D22AC689}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+      <selection activeCell="Q6" sqref="Q6:AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,52 +1020,52 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>